<commit_message>
added runtimes for classic and divide and conquer
</commit_message>
<xml_diff>
--- a/Advanced_Algorithms_Project_plan_EB-JR_JM-JB-AD_mid.xlsx
+++ b/Advanced_Algorithms_Project_plan_EB-JR_JM-JB-AD_mid.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9384" yWindow="0" windowWidth="27636" windowHeight="13020"/>
+    <workbookView xWindow="9390" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -1383,53 +1383,53 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1442,8 +1442,36 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFAAC56D"/>
@@ -1693,25 +1721,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BQ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="36.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.75" style="2" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.25" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="2.77734375" style="1"/>
+    <col min="7" max="7" width="16.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="2.75" style="1"/>
     <col min="14" max="15" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="20" width="2.77734375" style="1"/>
-    <col min="21" max="22" width="2.77734375" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="27" width="2.77734375" style="1"/>
+    <col min="16" max="20" width="2.75" style="1"/>
+    <col min="21" max="22" width="2.75" style="1" hidden="1" customWidth="1"/>
+    <col min="23" max="27" width="2.75" style="1"/>
     <col min="28" max="28" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="0" hidden="1" customWidth="1"/>
     <col min="35" max="36" width="0" hidden="1" customWidth="1"/>
@@ -1721,7 +1749,7 @@
     <col min="63" max="64" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="3"/>
@@ -1732,7 +1760,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="107"/>
       <c r="C2" s="107"/>
       <c r="D2" s="108"/>
@@ -1742,85 +1770,85 @@
       <c r="H2" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="131"/>
-      <c r="N2" s="131"/>
-      <c r="O2" s="131"/>
-      <c r="P2" s="131"/>
-      <c r="Q2" s="131"/>
-      <c r="R2" s="131"/>
-      <c r="S2" s="131"/>
-      <c r="T2" s="131"/>
-      <c r="U2" s="131"/>
-      <c r="V2" s="131"/>
-      <c r="W2" s="131"/>
-      <c r="X2" s="130" t="s">
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="137"/>
+      <c r="N2" s="137"/>
+      <c r="O2" s="137"/>
+      <c r="P2" s="137"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="137"/>
+      <c r="S2" s="137"/>
+      <c r="T2" s="137"/>
+      <c r="U2" s="137"/>
+      <c r="V2" s="137"/>
+      <c r="W2" s="137"/>
+      <c r="X2" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="131"/>
-      <c r="Z2" s="131"/>
-      <c r="AA2" s="131"/>
-      <c r="AB2" s="131"/>
-      <c r="AC2" s="131"/>
-      <c r="AD2" s="131"/>
-      <c r="AE2" s="131"/>
-      <c r="AF2" s="131"/>
-      <c r="AG2" s="131"/>
-      <c r="AH2" s="131"/>
-      <c r="AI2" s="131"/>
-      <c r="AJ2" s="131"/>
-      <c r="AK2" s="131"/>
-      <c r="AL2" s="131"/>
-      <c r="AM2" s="131"/>
-      <c r="AN2" s="131"/>
-      <c r="AO2" s="131"/>
-      <c r="AP2" s="131"/>
-      <c r="AQ2" s="131"/>
-      <c r="AR2" s="131"/>
-      <c r="AS2" s="131"/>
-      <c r="AT2" s="131"/>
-      <c r="AU2" s="131"/>
-      <c r="AV2" s="131"/>
-      <c r="AW2" s="131"/>
-      <c r="AX2" s="131"/>
-      <c r="AY2" s="131"/>
-      <c r="AZ2" s="131"/>
-      <c r="BA2" s="132"/>
-      <c r="BB2" s="131" t="s">
+      <c r="Y2" s="137"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="137"/>
+      <c r="AB2" s="137"/>
+      <c r="AC2" s="137"/>
+      <c r="AD2" s="137"/>
+      <c r="AE2" s="137"/>
+      <c r="AF2" s="137"/>
+      <c r="AG2" s="137"/>
+      <c r="AH2" s="137"/>
+      <c r="AI2" s="137"/>
+      <c r="AJ2" s="137"/>
+      <c r="AK2" s="137"/>
+      <c r="AL2" s="137"/>
+      <c r="AM2" s="137"/>
+      <c r="AN2" s="137"/>
+      <c r="AO2" s="137"/>
+      <c r="AP2" s="137"/>
+      <c r="AQ2" s="137"/>
+      <c r="AR2" s="137"/>
+      <c r="AS2" s="137"/>
+      <c r="AT2" s="137"/>
+      <c r="AU2" s="137"/>
+      <c r="AV2" s="137"/>
+      <c r="AW2" s="137"/>
+      <c r="AX2" s="137"/>
+      <c r="AY2" s="137"/>
+      <c r="AZ2" s="137"/>
+      <c r="BA2" s="138"/>
+      <c r="BB2" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="BC2" s="131"/>
-      <c r="BD2" s="131"/>
-      <c r="BE2" s="131"/>
-      <c r="BF2" s="131"/>
-      <c r="BG2" s="131"/>
-      <c r="BH2" s="131"/>
-      <c r="BI2" s="131"/>
-      <c r="BJ2" s="131"/>
-      <c r="BK2" s="131"/>
-      <c r="BL2" s="131"/>
-      <c r="BM2" s="131"/>
-      <c r="BN2" s="131"/>
-      <c r="BO2" s="131"/>
-      <c r="BP2" s="131"/>
-      <c r="BQ2" s="132"/>
+      <c r="BC2" s="137"/>
+      <c r="BD2" s="137"/>
+      <c r="BE2" s="137"/>
+      <c r="BF2" s="137"/>
+      <c r="BG2" s="137"/>
+      <c r="BH2" s="137"/>
+      <c r="BI2" s="137"/>
+      <c r="BJ2" s="137"/>
+      <c r="BK2" s="137"/>
+      <c r="BL2" s="137"/>
+      <c r="BM2" s="137"/>
+      <c r="BN2" s="137"/>
+      <c r="BO2" s="137"/>
+      <c r="BP2" s="137"/>
+      <c r="BQ2" s="138"/>
     </row>
-    <row r="3" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="107"/>
       <c r="C3" s="107"/>
-      <c r="D3" s="133" t="s">
+      <c r="D3" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="134"/>
-      <c r="F3" s="133" t="s">
+      <c r="E3" s="140"/>
+      <c r="F3" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="134"/>
+      <c r="G3" s="140"/>
       <c r="H3" s="109" t="s">
         <v>10</v>
       </c>
@@ -2008,7 +2036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="110" t="s">
         <v>16</v>
       </c>
@@ -2214,8 +2242,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="135" t="s">
+    <row r="5" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="128" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="123" t="s">
@@ -2259,7 +2287,7 @@
       <c r="AI5" s="19"/>
       <c r="AJ5" s="19"/>
       <c r="AK5" s="19"/>
-      <c r="AL5" s="137"/>
+      <c r="AL5" s="129"/>
       <c r="AM5" s="19"/>
       <c r="AN5" s="19"/>
       <c r="AO5" s="19"/>
@@ -2292,8 +2320,8 @@
       <c r="BP5" s="21"/>
       <c r="BQ5" s="23"/>
     </row>
-    <row r="6" spans="2:69" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="135" t="s">
+    <row r="6" spans="2:69" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="128" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="123" t="s">
@@ -2308,7 +2336,9 @@
       <c r="F6" s="28">
         <v>42661</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="14">
+        <v>3</v>
+      </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="50"/>
@@ -2339,7 +2369,7 @@
       <c r="AI6" s="19"/>
       <c r="AJ6" s="19"/>
       <c r="AK6" s="19"/>
-      <c r="AL6" s="137"/>
+      <c r="AL6" s="129"/>
       <c r="AM6" s="19"/>
       <c r="AN6" s="19"/>
       <c r="AO6" s="19"/>
@@ -2372,8 +2402,8 @@
       <c r="BP6" s="22"/>
       <c r="BQ6" s="24"/>
     </row>
-    <row r="7" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="135" t="s">
+    <row r="7" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="128" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="123" t="s">
@@ -2417,7 +2447,7 @@
       <c r="AI7" s="19"/>
       <c r="AJ7" s="19"/>
       <c r="AK7" s="19"/>
-      <c r="AL7" s="137"/>
+      <c r="AL7" s="129"/>
       <c r="AM7" s="19"/>
       <c r="AN7" s="19"/>
       <c r="AO7" s="19"/>
@@ -2450,7 +2480,7 @@
       <c r="BP7" s="22"/>
       <c r="BQ7" s="24"/>
     </row>
-    <row r="8" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="91" t="s">
         <v>21</v>
       </c>
@@ -2463,8 +2493,12 @@
       <c r="E8" s="14">
         <v>14</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
+      <c r="F8" s="28">
+        <v>42689</v>
+      </c>
+      <c r="G8" s="14">
+        <v>4</v>
+      </c>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -2495,7 +2529,7 @@
       <c r="AI8" s="48"/>
       <c r="AJ8" s="47"/>
       <c r="AK8" s="19"/>
-      <c r="AL8" s="137"/>
+      <c r="AL8" s="129"/>
       <c r="AM8" s="19"/>
       <c r="AN8" s="19"/>
       <c r="AO8" s="19"/>
@@ -2528,8 +2562,8 @@
       <c r="BP8" s="22"/>
       <c r="BQ8" s="24"/>
     </row>
-    <row r="9" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="135" t="s">
+    <row r="9" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="128" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="123" t="s">
@@ -2573,7 +2607,7 @@
       <c r="AI9" s="59"/>
       <c r="AJ9" s="59"/>
       <c r="AK9" s="59"/>
-      <c r="AL9" s="138"/>
+      <c r="AL9" s="130"/>
       <c r="AM9" s="59"/>
       <c r="AN9" s="59"/>
       <c r="AO9" s="60"/>
@@ -2608,8 +2642,8 @@
       <c r="BP9" s="22"/>
       <c r="BQ9" s="24"/>
     </row>
-    <row r="10" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="135" t="s">
+    <row r="10" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="128" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="123" t="s">
@@ -2655,7 +2689,7 @@
       <c r="AI10" s="19"/>
       <c r="AJ10" s="19"/>
       <c r="AK10" s="19"/>
-      <c r="AL10" s="137"/>
+      <c r="AL10" s="129"/>
       <c r="AM10" s="19"/>
       <c r="AN10" s="19"/>
       <c r="AO10" s="19"/>
@@ -2688,8 +2722,8 @@
       <c r="BP10" s="22"/>
       <c r="BQ10" s="24"/>
     </row>
-    <row r="11" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="128" t="s">
+    <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="141" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="123" t="s">
@@ -2733,7 +2767,7 @@
       <c r="AI11" s="19"/>
       <c r="AJ11" s="19"/>
       <c r="AK11" s="64"/>
-      <c r="AL11" s="139"/>
+      <c r="AL11" s="131"/>
       <c r="AM11" s="65"/>
       <c r="AN11" s="65"/>
       <c r="AO11" s="65"/>
@@ -2766,8 +2800,8 @@
       <c r="BP11" s="22"/>
       <c r="BQ11" s="24"/>
     </row>
-    <row r="12" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="128"/>
+    <row r="12" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="141"/>
       <c r="C12" s="123" t="s">
         <v>33</v>
       </c>
@@ -2775,7 +2809,9 @@
         <v>42688</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="28">
+        <v>42699</v>
+      </c>
       <c r="G12" s="14"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -2807,7 +2843,7 @@
       <c r="AI12" s="19"/>
       <c r="AJ12" s="19"/>
       <c r="AK12" s="51"/>
-      <c r="AL12" s="140"/>
+      <c r="AL12" s="132"/>
       <c r="AM12" s="52"/>
       <c r="AN12" s="52"/>
       <c r="AO12" s="52"/>
@@ -2840,8 +2876,8 @@
       <c r="BP12" s="22"/>
       <c r="BQ12" s="24"/>
     </row>
-    <row r="13" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="128" t="s">
+    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="141" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="123" t="s">
@@ -2885,7 +2921,7 @@
       <c r="AI13" s="19"/>
       <c r="AJ13" s="19"/>
       <c r="AK13" s="19"/>
-      <c r="AL13" s="137"/>
+      <c r="AL13" s="129"/>
       <c r="AM13" s="19"/>
       <c r="AN13" s="19"/>
       <c r="AO13" s="19"/>
@@ -2918,8 +2954,8 @@
       <c r="BP13" s="22"/>
       <c r="BQ13" s="24"/>
     </row>
-    <row r="14" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="128"/>
+    <row r="14" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="141"/>
       <c r="C14" s="123" t="s">
         <v>33</v>
       </c>
@@ -2927,8 +2963,12 @@
         <v>42667</v>
       </c>
       <c r="E14" s="14"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
+      <c r="F14" s="28">
+        <v>42679</v>
+      </c>
+      <c r="G14" s="14">
+        <v>4</v>
+      </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -2959,7 +2999,7 @@
       <c r="AI14" s="19"/>
       <c r="AJ14" s="19"/>
       <c r="AK14" s="19"/>
-      <c r="AL14" s="137"/>
+      <c r="AL14" s="129"/>
       <c r="AM14" s="19"/>
       <c r="AN14" s="19"/>
       <c r="AO14" s="19"/>
@@ -2992,8 +3032,8 @@
       <c r="BP14" s="22"/>
       <c r="BQ14" s="24"/>
     </row>
-    <row r="15" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="128" t="s">
+    <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="141" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="123" t="s">
@@ -3039,7 +3079,7 @@
       <c r="AK15" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="AL15" s="137"/>
+      <c r="AL15" s="129"/>
       <c r="AM15" s="19"/>
       <c r="AN15" s="19"/>
       <c r="AO15" s="19"/>
@@ -3072,8 +3112,8 @@
       <c r="BP15" s="22"/>
       <c r="BQ15" s="24"/>
     </row>
-    <row r="16" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="128"/>
+    <row r="16" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="141"/>
       <c r="C16" s="123" t="s">
         <v>34</v>
       </c>
@@ -3113,7 +3153,7 @@
       <c r="AI16" s="46"/>
       <c r="AJ16" s="46"/>
       <c r="AK16" s="19"/>
-      <c r="AL16" s="137"/>
+      <c r="AL16" s="129"/>
       <c r="AM16" s="19"/>
       <c r="AN16" s="19"/>
       <c r="AO16" s="19"/>
@@ -3146,8 +3186,8 @@
       <c r="BP16" s="22"/>
       <c r="BQ16" s="24"/>
     </row>
-    <row r="17" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="136" t="s">
+    <row r="17" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="143" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="123" t="s">
@@ -3191,7 +3231,7 @@
       <c r="AI17" s="19"/>
       <c r="AJ17" s="19"/>
       <c r="AK17" s="19"/>
-      <c r="AL17" s="137"/>
+      <c r="AL17" s="129"/>
       <c r="AM17" s="19"/>
       <c r="AN17" s="19"/>
       <c r="AO17" s="19"/>
@@ -3224,8 +3264,8 @@
       <c r="BP17" s="22"/>
       <c r="BQ17" s="24"/>
     </row>
-    <row r="18" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="136"/>
+    <row r="18" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="143"/>
       <c r="C18" s="123" t="s">
         <v>43</v>
       </c>
@@ -3265,7 +3305,7 @@
       <c r="AI18" s="19"/>
       <c r="AJ18" s="19"/>
       <c r="AK18" s="19"/>
-      <c r="AL18" s="137"/>
+      <c r="AL18" s="129"/>
       <c r="AM18" s="19"/>
       <c r="AN18" s="19"/>
       <c r="AO18" s="19"/>
@@ -3298,8 +3338,8 @@
       <c r="BP18" s="22"/>
       <c r="BQ18" s="24"/>
     </row>
-    <row r="19" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="128" t="s">
+    <row r="19" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="141" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="123" t="s">
@@ -3343,7 +3383,7 @@
       <c r="AI19" s="70"/>
       <c r="AJ19" s="70"/>
       <c r="AK19" s="70"/>
-      <c r="AL19" s="141"/>
+      <c r="AL19" s="133"/>
       <c r="AM19" s="70"/>
       <c r="AN19" s="70"/>
       <c r="AO19" s="71"/>
@@ -3378,8 +3418,8 @@
       <c r="BP19" s="22"/>
       <c r="BQ19" s="24"/>
     </row>
-    <row r="20" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="128"/>
+    <row r="20" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="141"/>
       <c r="C20" s="123" t="s">
         <v>36</v>
       </c>
@@ -3419,7 +3459,7 @@
       <c r="AI20" s="86"/>
       <c r="AJ20" s="86"/>
       <c r="AK20" s="86"/>
-      <c r="AL20" s="142"/>
+      <c r="AL20" s="134"/>
       <c r="AM20" s="86"/>
       <c r="AN20" s="86"/>
       <c r="AO20" s="87"/>
@@ -3452,7 +3492,7 @@
       <c r="BP20" s="22"/>
       <c r="BQ20" s="24"/>
     </row>
-    <row r="21" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="91" t="s">
         <v>29</v>
       </c>
@@ -3497,7 +3537,7 @@
       <c r="AI21" s="19"/>
       <c r="AJ21" s="19"/>
       <c r="AK21" s="19"/>
-      <c r="AL21" s="137"/>
+      <c r="AL21" s="129"/>
       <c r="AM21" s="19"/>
       <c r="AN21" s="19"/>
       <c r="AO21" s="19"/>
@@ -3530,7 +3570,7 @@
       <c r="BP21" s="22"/>
       <c r="BQ21" s="24"/>
     </row>
-    <row r="22" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="91" t="s">
         <v>30</v>
       </c>
@@ -3575,7 +3615,7 @@
       <c r="AI22" s="19"/>
       <c r="AJ22" s="19"/>
       <c r="AK22" s="19"/>
-      <c r="AL22" s="137"/>
+      <c r="AL22" s="129"/>
       <c r="AM22" s="19"/>
       <c r="AN22" s="19"/>
       <c r="AO22" s="19"/>
@@ -3608,8 +3648,8 @@
       <c r="BP22" s="22"/>
       <c r="BQ22" s="24"/>
     </row>
-    <row r="23" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="128" t="s">
+    <row r="23" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="141" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="123" t="s">
@@ -3621,7 +3661,9 @@
       <c r="E23" s="14">
         <v>14</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="28">
+        <v>42702</v>
+      </c>
       <c r="G23" s="14"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
@@ -3653,7 +3695,7 @@
       <c r="AI23" s="19"/>
       <c r="AJ23" s="19"/>
       <c r="AK23" s="19"/>
-      <c r="AL23" s="137"/>
+      <c r="AL23" s="129"/>
       <c r="AM23" s="19"/>
       <c r="AN23" s="19"/>
       <c r="AO23" s="19"/>
@@ -3686,8 +3728,8 @@
       <c r="BP23" s="22"/>
       <c r="BQ23" s="24"/>
     </row>
-    <row r="24" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="128"/>
+    <row r="24" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="141"/>
       <c r="C24" s="123" t="s">
         <v>35</v>
       </c>
@@ -3729,7 +3771,7 @@
       <c r="AI24" s="19"/>
       <c r="AJ24" s="19"/>
       <c r="AK24" s="19"/>
-      <c r="AL24" s="137"/>
+      <c r="AL24" s="129"/>
       <c r="AM24" s="19"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
@@ -3762,8 +3804,8 @@
       <c r="BP24" s="22"/>
       <c r="BQ24" s="24"/>
     </row>
-    <row r="25" spans="2:69" ht="18.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="128"/>
+    <row r="25" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="141"/>
       <c r="C25" s="123" t="s">
         <v>43</v>
       </c>
@@ -3805,7 +3847,7 @@
       <c r="AI25" s="19"/>
       <c r="AJ25" s="19"/>
       <c r="AK25" s="19"/>
-      <c r="AL25" s="137"/>
+      <c r="AL25" s="129"/>
       <c r="AM25" s="19"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
@@ -3838,8 +3880,8 @@
       <c r="BP25" s="22"/>
       <c r="BQ25" s="24"/>
     </row>
-    <row r="26" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="128" t="s">
+    <row r="26" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="141" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="123" t="s">
@@ -3883,7 +3925,7 @@
       <c r="AI26" s="19"/>
       <c r="AJ26" s="19"/>
       <c r="AK26" s="19"/>
-      <c r="AL26" s="137"/>
+      <c r="AL26" s="129"/>
       <c r="AM26" s="19"/>
       <c r="AN26" s="19"/>
       <c r="AO26" s="19"/>
@@ -3916,8 +3958,8 @@
       <c r="BP26" s="22"/>
       <c r="BQ26" s="24"/>
     </row>
-    <row r="27" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="129"/>
+    <row r="27" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="142"/>
       <c r="C27" s="124" t="s">
         <v>36</v>
       </c>
@@ -3959,7 +4001,7 @@
       <c r="AI27" s="30"/>
       <c r="AJ27" s="30"/>
       <c r="AK27" s="30"/>
-      <c r="AL27" s="143"/>
+      <c r="AL27" s="135"/>
       <c r="AM27" s="30"/>
       <c r="AN27" s="30"/>
       <c r="AO27" s="30"/>
@@ -3992,7 +4034,7 @@
       <c r="BP27" s="25"/>
       <c r="BQ27" s="26"/>
     </row>
-    <row r="29" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B29" s="37" t="s">
         <v>37</v>
       </c>
@@ -4000,25 +4042,25 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B30" s="38"/>
       <c r="C30" s="41" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B31" s="38"/>
       <c r="C31" s="42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B32" s="38"/>
       <c r="C32" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="39"/>
       <c r="C33" s="44" t="s">
         <v>34</v>
@@ -4027,11 +4069,6 @@
   </sheetData>
   <autoFilter ref="B4:G27"/>
   <mergeCells count="12">
-    <mergeCell ref="I2:W2"/>
-    <mergeCell ref="X2:BA2"/>
-    <mergeCell ref="BB2:BQ2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B13:B14"/>
@@ -4039,6 +4076,11 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B23:B25"/>
+    <mergeCell ref="I2:W2"/>
+    <mergeCell ref="X2:BA2"/>
+    <mergeCell ref="BB2:BQ2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>